<commit_message>
few changes to make error message professional, and submit button cooler. Added some support for non abbreviations
</commit_message>
<xml_diff>
--- a/abbreviations.xlsx
+++ b/abbreviations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devan\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810937FF-9BDE-4D69-B8C1-F12EB645F728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EA4B10-3C39-4B94-B16E-32C74E747314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{509D3843-75A1-4BFF-AAC8-91F52D8E0F9C}"/>
   </bookViews>
@@ -1353,9 +1353,6 @@
     <t>It sends provisioning (update) instructions (in the form of XML files) via IB Production Broker to an Activator Agents process on the target hosts.|PE provisions via IB:|-MDB.  This data includes Service, CUG, MRR and MVAL. Also see AA, ACL &amp; SOPIE|-Master ED.  This data includes SNL configuration, system configuration, etc.|-SnF (ISQ).  This data includes queues created on behalf of customers.|-SMS.</t>
   </si>
   <si>
-    <t xml:space="preserve">Perl </t>
-  </si>
-  <si>
     <t xml:space="preserve">Scripting &amp; programming software / shell </t>
   </si>
   <si>
@@ -2075,6 +2072,9 @@
   </si>
   <si>
     <t>TACACS</t>
+  </si>
+  <si>
+    <t>PERL</t>
   </si>
 </sst>
 </file>
@@ -2518,24 +2518,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27586D9F-C034-45D5-B57A-BC15E14CA00C}">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>607</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>608</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
@@ -4504,7 +4504,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A143" s="5" t="s">
-        <v>379</v>
+        <v>610</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>31</v>
@@ -4513,85 +4513,85 @@
         <v>156</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A144" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B144" s="6" t="s">
         <v>381</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>382</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A145" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B145" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A146" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B146" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A147" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B147" s="6" t="s">
         <v>390</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>391</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A148" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B148" s="6" t="s">
         <v>393</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>394</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A149" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B149" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="B149" s="6" t="s">
-        <v>397</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>18</v>
@@ -4600,105 +4600,105 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A150" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B150" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A151" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B151" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A152" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B152" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A153" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B153" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>408</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A154" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B154" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A155" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B155" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="B155" s="6" t="s">
+      <c r="C155" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="C155" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A156" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B156" s="6" t="s">
         <v>416</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>417</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A157" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>31</v>
@@ -4712,108 +4712,108 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A158" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B158" s="6" t="s">
         <v>420</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>421</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A159" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B159" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A160" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B160" s="6" t="s">
         <v>426</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>427</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A161" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B161" s="6" t="s">
         <v>429</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>430</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A162" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B162" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="C162" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D162" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A163" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B163" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>436</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A164" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B164" s="6" t="s">
         <v>438</v>
-      </c>
-      <c r="B164" s="6" t="s">
-        <v>439</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A165" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B165" s="6" t="s">
         <v>441</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>3</v>
@@ -4824,10 +4824,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A166" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B166" s="6" t="s">
         <v>443</v>
-      </c>
-      <c r="B166" s="6" t="s">
-        <v>444</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>57</v>
@@ -4838,24 +4838,24 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A167" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B167" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="C167" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" s="6" t="s">
         <v>446</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D167" s="6" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A168" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B168" s="6" t="s">
         <v>448</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>449</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>156</v>
@@ -4866,10 +4866,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A169" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B169" s="6" t="s">
         <v>450</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>451</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>31</v>
@@ -4880,52 +4880,52 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A170" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B170" s="6" t="s">
         <v>452</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A171" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B171" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A172" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B172" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="B172" s="6" t="s">
+      <c r="C172" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A173" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="B173" s="6" t="s">
         <v>461</v>
-      </c>
-      <c r="B173" s="6" t="s">
-        <v>462</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>31</v>
@@ -4936,24 +4936,24 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A174" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B174" s="6" t="s">
         <v>463</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>464</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A175" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B175" s="6" t="s">
         <v>466</v>
-      </c>
-      <c r="B175" s="6" t="s">
-        <v>467</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>57</v>
@@ -4964,10 +4964,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A176" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B176" s="6" t="s">
         <v>468</v>
-      </c>
-      <c r="B176" s="6" t="s">
-        <v>469</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>57</v>
@@ -4978,10 +4978,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A177" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B177" s="6" t="s">
         <v>470</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>471</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>57</v>
@@ -4992,24 +4992,24 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A178" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B178" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="B178" s="6" t="s">
+      <c r="C178" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="6" t="s">
         <v>473</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D178" s="6" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A179" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B179" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>476</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>3</v>
@@ -5020,10 +5020,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A180" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B180" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="B180" s="6" t="s">
-        <v>478</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>31</v>
@@ -5034,10 +5034,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A181" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B181" s="6" t="s">
         <v>479</v>
-      </c>
-      <c r="B181" s="6" t="s">
-        <v>480</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>31</v>
@@ -5048,10 +5048,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A182" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B182" s="6" t="s">
         <v>481</v>
-      </c>
-      <c r="B182" s="6" t="s">
-        <v>482</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>31</v>
@@ -5062,24 +5062,24 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A183" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B183" s="6" t="s">
         <v>483</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>484</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A184" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B184" s="6" t="s">
         <v>486</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>487</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>3</v>
@@ -5090,38 +5090,38 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A185" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B185" s="6" t="s">
         <v>488</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>489</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A186" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B186" s="6" t="s">
         <v>491</v>
-      </c>
-      <c r="B186" s="6" t="s">
-        <v>492</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A187" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B187" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="B187" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>34</v>
@@ -5130,10 +5130,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A188" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B188" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>3</v>
@@ -5144,94 +5144,94 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A189" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B189" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="C189" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D189" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="C189" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D189" s="6" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A190" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B190" s="6" t="s">
         <v>501</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>502</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A191" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="B191" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="C191" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D191" s="6" t="s">
         <v>505</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D191" s="6" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A192" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B192" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A193" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B193" s="9" t="s">
         <v>510</v>
       </c>
-      <c r="B193" s="9" t="s">
+      <c r="C193" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D193" s="9" t="s">
         <v>511</v>
-      </c>
-      <c r="C193" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A194" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B194" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="B194" s="6" t="s">
+      <c r="C194" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" s="6" t="s">
         <v>514</v>
-      </c>
-      <c r="C194" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D194" s="6" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A195" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>57</v>
@@ -5242,10 +5242,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A196" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B196" s="6" t="s">
         <v>517</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>518</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>31</v>
@@ -5256,24 +5256,24 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A197" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B197" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>520</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A198" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>522</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>523</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>31</v>
@@ -5284,10 +5284,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A199" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="B199" s="6" t="s">
         <v>524</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>525</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>31</v>
@@ -5298,38 +5298,38 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A200" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B200" s="6" t="s">
         <v>526</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>527</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A201" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B201" s="6" t="s">
         <v>529</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>530</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A202" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B202" s="6" t="s">
         <v>532</v>
-      </c>
-      <c r="B202" s="6" t="s">
-        <v>533</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>3</v>
@@ -5340,10 +5340,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A203" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B203" s="6" t="s">
         <v>534</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>535</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>3</v>
@@ -5354,7 +5354,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A204" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>31</v>
@@ -5368,13 +5368,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A205" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B205" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B205" s="6" t="s">
+      <c r="C205" s="6" t="s">
         <v>537</v>
-      </c>
-      <c r="C205" s="6" t="s">
-        <v>538</v>
       </c>
       <c r="D205" s="6" t="s">
         <v>31</v>
@@ -5382,10 +5382,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A206" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="B206" s="6" t="s">
         <v>539</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>540</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>3</v>
@@ -5396,16 +5396,16 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A207" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B207" s="6" t="s">
         <v>541</v>
-      </c>
-      <c r="B207" s="6" t="s">
-        <v>542</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.75">
@@ -5413,35 +5413,35 @@
         <v>18</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A209" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="B209" s="6" t="s">
         <v>545</v>
-      </c>
-      <c r="B209" s="6" t="s">
-        <v>546</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A210" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B210" s="6" t="s">
         <v>548</v>
-      </c>
-      <c r="B210" s="6" t="s">
-        <v>549</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>3</v>
@@ -5452,38 +5452,38 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A211" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="B211" s="6" t="s">
         <v>550</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>551</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A212" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B212" s="6" t="s">
         <v>553</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>554</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A213" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="B213" s="6" t="s">
         <v>556</v>
-      </c>
-      <c r="B213" s="6" t="s">
-        <v>557</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>3</v>
@@ -5494,80 +5494,80 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A214" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="B214" s="6" t="s">
         <v>558</v>
-      </c>
-      <c r="B214" s="6" t="s">
-        <v>559</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A215" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D215" s="6" t="s">
         <v>561</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D215" s="6" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A216" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B216" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="B216" s="6" t="s">
+      <c r="C216" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D216" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="C216" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D216" s="6" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A217" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B217" s="6" t="s">
         <v>566</v>
-      </c>
-      <c r="B217" s="6" t="s">
-        <v>567</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A218" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="B218" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="B218" s="6" t="s">
+      <c r="C218" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D218" s="6" t="s">
         <v>570</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D218" s="6" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A219" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B219" s="6" t="s">
         <v>572</v>
-      </c>
-      <c r="B219" s="6" t="s">
-        <v>573</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>3</v>
@@ -5578,38 +5578,38 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A220" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B220" s="6" t="s">
         <v>574</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>575</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>365</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A221" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B221" s="6" t="s">
         <v>577</v>
       </c>
-      <c r="B221" s="6" t="s">
+      <c r="C221" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="D221" s="6" t="s">
         <v>578</v>
-      </c>
-      <c r="C221" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="D221" s="6" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A222" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B222" s="6" t="s">
         <v>580</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>581</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>3</v>
@@ -5620,10 +5620,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A223" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="B223" s="6" t="s">
         <v>582</v>
-      </c>
-      <c r="B223" s="6" t="s">
-        <v>583</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>57</v>
@@ -5634,7 +5634,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A224" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>31</v>
@@ -5643,57 +5643,57 @@
         <v>57</v>
       </c>
       <c r="D224" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A225" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="B225" s="6" t="s">
         <v>586</v>
-      </c>
-      <c r="B225" s="6" t="s">
-        <v>587</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A226" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B226" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="B226" s="6" t="s">
+      <c r="C226" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D226" s="6" t="s">
         <v>590</v>
-      </c>
-      <c r="C226" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D226" s="6" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A227" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B227" s="6" t="s">
         <v>592</v>
-      </c>
-      <c r="B227" s="6" t="s">
-        <v>593</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A228" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="B228" s="6" t="s">
         <v>595</v>
-      </c>
-      <c r="B228" s="6" t="s">
-        <v>596</v>
       </c>
       <c r="C228" s="6" t="s">
         <v>3</v>
@@ -5704,24 +5704,24 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A229" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A230" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="B230" s="6" t="s">
         <v>599</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>600</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>57</v>
@@ -5732,10 +5732,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A231" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="B231" s="6" t="s">
         <v>601</v>
-      </c>
-      <c r="B231" s="6" t="s">
-        <v>602</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>3</v>
@@ -5746,10 +5746,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A232" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B232" s="6" t="s">
         <v>603</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>604</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>3</v>
@@ -5760,10 +5760,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A233" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B233" s="6" t="s">
         <v>605</v>
-      </c>
-      <c r="B233" s="6" t="s">
-        <v>606</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
final push i swear
</commit_message>
<xml_diff>
--- a/abbreviations.xlsx
+++ b/abbreviations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devan\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EA4B10-3C39-4B94-B16E-32C74E747314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56330D8A-F0CC-4761-B125-BABD681F7F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{509D3843-75A1-4BFF-AAC8-91F52D8E0F9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="612">
   <si>
     <t>Relation to</t>
   </si>
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t>Cluster</t>
-  </si>
-  <si>
-    <t>Name of concept</t>
   </si>
   <si>
     <t>A cluster can consist of 1 to 8 nodes. A cluster is a grouping of hosts used to run the same software for contingency. Can run in active/active or active/standby mode. Active/Active: All hosts in the cluster run the application at the same time. Active/Standby: Only one host runs the application, other hosts in the cluster are up running, in case the application has to be moved.||Major benefits of a cluster:|-High availability of applications running on these nodes|-Minimizes down time.|-The cluster can be used for rolling upgrades.||Used for Cluster Management:|-Application or Package is hosted on one machine.|-Another machine is loaded and configured exactly as the first.|-When a problem is detected the application is swovered (acronym for switched over).|-Swovers can be automatic or operator initiated.|-Clusters are used for resiliency and contingency purposes.||Swift Clusters uses: |-Mirrored disk drives in the hosts.|-Shared file systems on XP512 systems use Raid disk drives.|-MC Service Guard application must be running on the node before the PKG||Software failures:|-Application can be restarted on same machine.|-Application can be switched over to another machine within cluster.|-If pkg switching is enabled then the application is automatically brought up on the standby cluster host</t>
@@ -1500,9 +1497,6 @@
     <t>Memo of the IETF on a specific subject.</t>
   </si>
   <si>
-    <t xml:space="preserve">RMAN </t>
-  </si>
-  <si>
     <t xml:space="preserve">Recovery Manager </t>
   </si>
   <si>
@@ -1805,9 +1799,6 @@
   </si>
   <si>
     <t xml:space="preserve">Society for Worldwide Interbank Financial Telecommunication </t>
-  </si>
-  <si>
-    <t>SWIFT is the industry-owned cooperative supplying secure messaging services and interface Software to 7,000 financial institutions in 197 countries. Its services help Customers reduce costs, improve automation and manage risk. The overall SWIFT strategy is to deliver 5 channels of value to our customers and the financial industry, being:  Resilience, Single window, Pricing, Standards, STP (Straight Through Processing).</t>
   </si>
   <si>
     <t>SWOVER</t>
@@ -2075,6 +2066,18 @@
   </si>
   <si>
     <t>PERL</t>
+  </si>
+  <si>
+    <t>RMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIFT is the industry-owned cooperative supplying secure messaging services and interface Software to 7,000 financial institutions in 197 countries. Its services help Customers reduce costs, improve automation and manage risk. </t>
+  </si>
+  <si>
+    <t>The overall SWIFT strategy is to deliver 5 channels of value to our customers and the financial industry, being:  Resilience, Single window, Pricing, Standards, STP (Straight Through Processing).</t>
+  </si>
+  <si>
+    <t>CRS-COMP</t>
   </si>
 </sst>
 </file>
@@ -2516,26 +2519,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27586D9F-C034-45D5-B57A-BC15E14CA00C}">
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:F247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="E192" sqref="E192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="35.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" s="13" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
@@ -3027,35 +3033,35 @@
         <v>102</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A39" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>34</v>
@@ -3066,27 +3072,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A40" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A41" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="C41" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>31</v>
@@ -3094,13 +3100,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A42" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="C42" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>31</v>
@@ -3108,10 +3114,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A43" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>18</v>
@@ -3122,10 +3128,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A44" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>34</v>
@@ -3136,108 +3142,108 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A45" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A46" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A47" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A48" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A49" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A50" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="C50" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A51" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A52" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>144</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>18</v>
@@ -3248,24 +3254,24 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A54" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>34</v>
@@ -3276,63 +3282,63 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A55" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="C55" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A56" s="5" t="s">
-        <v>148</v>
+        <v>611</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A57" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A58" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A59" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>31</v>
@@ -3341,29 +3347,29 @@
         <v>34</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A60" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A61" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>18</v>
@@ -3374,38 +3380,38 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A62" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A63" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="C63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A64" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>34</v>
@@ -3416,83 +3422,83 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A65" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A66" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A67" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="C67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A68" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="C68" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A69" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="C69" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A70" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="C70" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>31</v>
@@ -3500,80 +3506,80 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A71" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C71" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A72" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A73" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A74" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C74" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A75" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" s="12" t="s">
         <v>204</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>205</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A76" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>3</v>
@@ -3584,10 +3590,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A77" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>3</v>
@@ -3598,38 +3604,38 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A78" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A79" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A80" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>3</v>
@@ -3640,24 +3646,24 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A81" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="C81" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A82" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>57</v>
@@ -3668,21 +3674,21 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A83" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A84" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>31</v>
@@ -3696,80 +3702,80 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A85" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A86" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A87" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="C87" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D87" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A88" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C88" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A89" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="C89" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A90" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>18</v>
@@ -3780,41 +3786,41 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A91" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A92" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="C92" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A93" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>252</v>
-      </c>
       <c r="C93" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>31</v>
@@ -3822,10 +3828,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A94" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>31</v>
@@ -3836,24 +3842,24 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A95" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="C95" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A96" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>18</v>
@@ -3864,108 +3870,108 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A97" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="C97" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A98" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A99" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="C99" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A100" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A101" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="C101" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A102" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A103" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B103" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="C103" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A104" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>3</v>
@@ -3976,10 +3982,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A105" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>31</v>
@@ -3990,24 +3996,24 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A106" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A107" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>3</v>
@@ -4016,66 +4022,66 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A108" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="C108" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A109" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="C109" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A110" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A111" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="C111" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D111" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A112" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>3</v>
@@ -4084,38 +4090,38 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A113" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B113" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="C113" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A114" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B114" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="C114" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A115" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>18</v>
@@ -4126,24 +4132,24 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A116" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B116" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="C116" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D116" s="6" t="s">
         <v>313</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A117" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>3</v>
@@ -4154,24 +4160,24 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A118" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B118" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="C118" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D118" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A119" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B119" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>57</v>
@@ -4182,24 +4188,24 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A120" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B120" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>323</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A121" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B121" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>3</v>
@@ -4210,13 +4216,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A122" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>31</v>
@@ -4224,10 +4230,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A123" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>34</v>
@@ -4238,66 +4244,66 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A124" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B124" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A125" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>334</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A126" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B126" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="C126" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A127" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B127" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A128" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>18</v>
@@ -4308,80 +4314,80 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A129" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B129" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B129" s="6" t="s">
+      <c r="C129" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D129" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A130" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B130" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="C130" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D130" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A131" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B131" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="C131" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D131" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A132" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B132" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="C132" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D132" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A133" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D133" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A134" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B134" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>3</v>
@@ -4392,10 +4398,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A135" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B135" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>3</v>
@@ -4406,52 +4412,52 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A136" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B136" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="C136" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D136" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D136" s="6" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A137" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B137" s="6" t="s">
         <v>365</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A138" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B138" s="6" t="s">
         <v>368</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>369</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A139" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>31</v>
@@ -4462,7 +4468,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A140" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>31</v>
@@ -4476,122 +4482,122 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A141" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B141" s="6" t="s">
         <v>373</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>374</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A142" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B142" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="C142" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>377</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A143" s="5" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A144" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B144" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>381</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A145" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B145" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>384</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A146" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B146" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="B146" s="6" t="s">
+      <c r="C146" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D146" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D146" s="6" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A147" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B147" s="6" t="s">
         <v>389</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A148" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B148" s="6" t="s">
         <v>392</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>393</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A149" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B149" s="6" t="s">
         <v>395</v>
-      </c>
-      <c r="B149" s="6" t="s">
-        <v>396</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>18</v>
@@ -4600,111 +4606,111 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A150" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B150" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A151" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B151" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A152" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B152" s="6" t="s">
         <v>403</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>404</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A153" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B153" s="6" t="s">
         <v>406</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A154" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B154" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>410</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A155" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B155" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="B155" s="6" t="s">
+      <c r="C155" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="C155" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A156" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B156" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>416</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A157" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>31</v>
@@ -4712,108 +4718,108 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A158" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B158" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>420</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A159" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B159" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="C159" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D159" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D159" s="6" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A160" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B160" s="6" t="s">
         <v>425</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>426</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A161" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D161" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161" s="6" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A162" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D162" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A163" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A164" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A165" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>3</v>
@@ -4824,10 +4830,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A166" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>57</v>
@@ -4838,27 +4844,27 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A167" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" s="6" t="s">
         <v>444</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D167" s="6" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A168" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>31</v>
@@ -4866,10 +4872,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A169" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>31</v>
@@ -4880,52 +4886,52 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A170" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A171" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A172" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A173" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>31</v>
@@ -4936,24 +4942,24 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A174" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A175" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>57</v>
@@ -4964,10 +4970,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A176" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>57</v>
@@ -4978,10 +4984,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A177" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>57</v>
@@ -4992,24 +4998,24 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A178" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="6" t="s">
         <v>471</v>
-      </c>
-      <c r="B178" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D178" s="6" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A179" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>3</v>
@@ -5020,10 +5026,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A180" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>31</v>
@@ -5034,10 +5040,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A181" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>31</v>
@@ -5048,10 +5054,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A182" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>31</v>
@@ -5062,24 +5068,24 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A183" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A184" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>3</v>
@@ -5090,38 +5096,38 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A185" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A186" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A187" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>34</v>
@@ -5130,10 +5136,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A188" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>3</v>
@@ -5144,94 +5150,94 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A189" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D189" s="6" t="s">
         <v>497</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="C189" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D189" s="6" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A190" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A191" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D191" s="6" t="s">
         <v>503</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D191" s="6" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A192" s="5" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D192" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A193" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B193" s="9" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A193" s="5" t="s">
+      <c r="C193" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D193" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B193" s="9" t="s">
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A194" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="C193" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D193" s="9" t="s">
+      <c r="B194" s="6" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A194" s="5" t="s">
+      <c r="C194" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="B194" s="6" t="s">
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A195" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B195" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="C194" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D194" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A195" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="B195" s="6" t="s">
-        <v>515</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>57</v>
@@ -5240,208 +5246,211 @@
         <v>31</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A196" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A197" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="B196" s="6" t="s">
+      <c r="B197" s="6" t="s">
         <v>517</v>
-      </c>
-      <c r="C196" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A197" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>519</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D197" s="6" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A198" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A198" s="5" t="s">
+      <c r="C198" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D198" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A199" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="B198" s="6" t="s">
+      <c r="B199" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="C198" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D198" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A199" s="5" t="s">
+      <c r="C199" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D199" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F199" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A200" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="B199" s="6" t="s">
+      <c r="B200" s="6" t="s">
         <v>524</v>
-      </c>
-      <c r="C199" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D199" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A200" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D200" s="6" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A201" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D201" s="6" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A201" s="5" t="s">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A202" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="B201" s="6" t="s">
+      <c r="B202" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="C201" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D201" s="6" t="s">
+      <c r="C202" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D202" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A203" s="5" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A202" s="5" t="s">
+      <c r="B203" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="B202" s="6" t="s">
+      <c r="C203" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D203" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A204" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C204" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A205" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="C202" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D202" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A203" s="5" t="s">
+      <c r="B205" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B203" s="6" t="s">
+      <c r="C205" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="C203" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D203" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A204" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="B204" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C204" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D204" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A205" s="5" t="s">
+      <c r="D205" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A206" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="B205" s="6" t="s">
+      <c r="B206" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="C205" s="6" t="s">
+      <c r="C206" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A207" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="D205" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A206" s="4" t="s">
+      <c r="B207" s="6" t="s">
         <v>538</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D206" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A207" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="B207" s="6" t="s">
-        <v>541</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.75">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A208" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A209" s="5" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A210" s="5" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>3</v>
@@ -5452,38 +5461,38 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A211" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A212" s="5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A213" s="5" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>3</v>
@@ -5494,21 +5503,21 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A214" s="5" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A215" s="5" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B215" s="6" t="s">
         <v>31</v>
@@ -5517,57 +5526,57 @@
         <v>3</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A216" s="5" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A217" s="5" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A218" s="5" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A219" s="5" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>3</v>
@@ -5578,38 +5587,38 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A220" s="5" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A221" s="5" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A222" s="5" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>3</v>
@@ -5620,10 +5629,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A223" s="5" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>57</v>
@@ -5634,7 +5643,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A224" s="5" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>31</v>
@@ -5643,57 +5652,57 @@
         <v>57</v>
       </c>
       <c r="D224" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A225" s="5" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A226" s="5" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C226" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D226" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A227" s="5" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A228" s="5" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C228" s="6" t="s">
         <v>3</v>
@@ -5704,24 +5713,24 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A229" s="5" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A230" s="5" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>57</v>
@@ -5732,10 +5741,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A231" s="5" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>3</v>
@@ -5746,10 +5755,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A232" s="5" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>3</v>
@@ -5760,10 +5769,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A233" s="5" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>3</v>

</xml_diff>